<commit_message>
more tests and modifications
</commit_message>
<xml_diff>
--- a/src/test/java/data/input.xlsx
+++ b/src/test/java/data/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliass\Desktop\Automation course\Involve.me\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D24827D-AC97-4D21-828A-5B32D04186B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA25193F-EABD-4220-A36D-62029E285E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B090ACDA-573D-4725-AF53-8BAC3CA59CC1}"/>
+    <workbookView xWindow="4050" yWindow="3000" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B090ACDA-573D-4725-AF53-8BAC3CA59CC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -62,13 +62,13 @@
     <t>jklJKLmicld</t>
   </si>
   <si>
-    <t>contact form</t>
-  </si>
-  <si>
-    <t>rating</t>
-  </si>
-  <si>
     <t>Elements</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Contact Form</t>
   </si>
 </sst>
 </file>
@@ -505,14 +505,14 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>